<commit_message>
IMPRESION MULTIPLE DE ETIQUETAS PARA GONDOLA
</commit_message>
<xml_diff>
--- a/CCFN-A003-A02.04 WORKFLOW AVISO DIFERENCIA COSTOS/CCFN-A003-A02.04-F010-R00 CASOS DE PRUEBA.xlsx
+++ b/CCFN-A003-A02.04 WORKFLOW AVISO DIFERENCIA COSTOS/CCFN-A003-A02.04-F010-R00 CASOS DE PRUEBA.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\OP Gerencia\Documents\CLAUDIA\PROYECTOS\003 WORKFLOW AVISO DIFERENCIA COSTOS\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SISTEMAS\Documents\GitHub\Proyectos\CCFN-A003-A02.04 WORKFLOW AVISO DIFERENCIA COSTOS\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -241,7 +241,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="00000"/>
   </numFmts>
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -280,6 +280,29 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="8"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -450,7 +473,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="64">
+  <cellXfs count="65">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -469,165 +492,166 @@
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="15" fontId="6" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="15" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -743,13 +767,13 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>3</xdr:col>
+      <xdr:col>2</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>1</xdr:row>
       <xdr:rowOff>114300</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>3</xdr:col>
+      <xdr:col>2</xdr:col>
       <xdr:colOff>771525</xdr:colOff>
       <xdr:row>3</xdr:row>
       <xdr:rowOff>114300</xdr:rowOff>
@@ -781,13 +805,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>9</xdr:col>
+      <xdr:col>8</xdr:col>
       <xdr:colOff>104775</xdr:colOff>
       <xdr:row>1</xdr:row>
       <xdr:rowOff>28575</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>9</xdr:col>
+      <xdr:col>8</xdr:col>
       <xdr:colOff>660400</xdr:colOff>
       <xdr:row>3</xdr:row>
       <xdr:rowOff>160020</xdr:rowOff>
@@ -1117,49 +1141,49 @@
     </row>
     <row r="2" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B2" s="1"/>
-      <c r="C2" s="17"/>
-      <c r="D2" s="20" t="s">
+      <c r="C2" s="16"/>
+      <c r="D2" s="19" t="s">
         <v>2</v>
       </c>
-      <c r="E2" s="20"/>
-      <c r="F2" s="20"/>
-      <c r="G2" s="21" t="s">
+      <c r="E2" s="19"/>
+      <c r="F2" s="19"/>
+      <c r="G2" s="20" t="s">
         <v>0</v>
       </c>
-      <c r="H2" s="16"/>
+      <c r="H2" s="15"/>
     </row>
     <row r="3" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B3" s="1"/>
-      <c r="C3" s="18"/>
-      <c r="D3" s="20"/>
-      <c r="E3" s="20"/>
-      <c r="F3" s="20"/>
-      <c r="G3" s="21"/>
-      <c r="H3" s="16"/>
+      <c r="C3" s="17"/>
+      <c r="D3" s="19"/>
+      <c r="E3" s="19"/>
+      <c r="F3" s="19"/>
+      <c r="G3" s="20"/>
+      <c r="H3" s="15"/>
     </row>
     <row r="4" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B4" s="1"/>
-      <c r="C4" s="19"/>
-      <c r="D4" s="20"/>
-      <c r="E4" s="20"/>
-      <c r="F4" s="20"/>
+      <c r="C4" s="18"/>
+      <c r="D4" s="19"/>
+      <c r="E4" s="19"/>
+      <c r="F4" s="19"/>
       <c r="G4" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="H4" s="16"/>
+      <c r="H4" s="15"/>
     </row>
     <row r="6" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B6" s="5"/>
-      <c r="C6" s="15" t="s">
+      <c r="C6" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="D6" s="15"/>
-      <c r="E6" s="15"/>
-      <c r="F6" s="15"/>
-      <c r="G6" s="15" t="s">
+      <c r="D6" s="11"/>
+      <c r="E6" s="11"/>
+      <c r="F6" s="11"/>
+      <c r="G6" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="H6" s="15"/>
+      <c r="H6" s="11"/>
       <c r="I6" s="5"/>
     </row>
     <row r="7" spans="2:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -1173,113 +1197,125 @@
       <c r="I7" s="8"/>
     </row>
     <row r="8" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B8" s="14" t="s">
+      <c r="B8" s="21" t="s">
         <v>5</v>
       </c>
-      <c r="C8" s="14"/>
-      <c r="D8" s="14"/>
-      <c r="E8" s="14"/>
-      <c r="F8" s="14"/>
-      <c r="G8" s="14" t="s">
+      <c r="C8" s="21"/>
+      <c r="D8" s="21"/>
+      <c r="E8" s="21"/>
+      <c r="F8" s="21"/>
+      <c r="G8" s="21" t="s">
         <v>6</v>
       </c>
-      <c r="H8" s="14"/>
-      <c r="I8" s="14"/>
+      <c r="H8" s="21"/>
+      <c r="I8" s="21"/>
     </row>
     <row r="9" spans="2:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="15" t="s">
+      <c r="B9" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="C9" s="15"/>
-      <c r="D9" s="15"/>
-      <c r="E9" s="15"/>
-      <c r="F9" s="15"/>
-      <c r="G9" s="15"/>
-      <c r="H9" s="15"/>
-      <c r="I9" s="15"/>
+      <c r="C9" s="11"/>
+      <c r="D9" s="11"/>
+      <c r="E9" s="11"/>
+      <c r="F9" s="11"/>
+      <c r="G9" s="11"/>
+      <c r="H9" s="11"/>
+      <c r="I9" s="11"/>
     </row>
     <row r="10" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B10" s="15" t="s">
+      <c r="B10" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="C10" s="15"/>
-      <c r="D10" s="15"/>
-      <c r="E10" s="15"/>
-      <c r="F10" s="15"/>
-      <c r="G10" s="15"/>
-      <c r="H10" s="15"/>
-      <c r="I10" s="15"/>
+      <c r="C10" s="11"/>
+      <c r="D10" s="11"/>
+      <c r="E10" s="11"/>
+      <c r="F10" s="11"/>
+      <c r="G10" s="11"/>
+      <c r="H10" s="11"/>
+      <c r="I10" s="11"/>
     </row>
     <row r="11" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B11" s="15" t="s">
+      <c r="B11" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="C11" s="15"/>
-      <c r="D11" s="15"/>
-      <c r="E11" s="15"/>
-      <c r="F11" s="15"/>
-      <c r="G11" s="15"/>
-      <c r="H11" s="15"/>
-      <c r="I11" s="15"/>
+      <c r="C11" s="11"/>
+      <c r="D11" s="11"/>
+      <c r="E11" s="11"/>
+      <c r="F11" s="11"/>
+      <c r="G11" s="11"/>
+      <c r="H11" s="11"/>
+      <c r="I11" s="11"/>
     </row>
     <row r="12" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B12" s="15" t="s">
+      <c r="B12" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="C12" s="15"/>
-      <c r="D12" s="15"/>
-      <c r="E12" s="15"/>
-      <c r="F12" s="15"/>
-      <c r="G12" s="15"/>
-      <c r="H12" s="15"/>
-      <c r="I12" s="15"/>
+      <c r="C12" s="11"/>
+      <c r="D12" s="11"/>
+      <c r="E12" s="11"/>
+      <c r="F12" s="11"/>
+      <c r="G12" s="11"/>
+      <c r="H12" s="11"/>
+      <c r="I12" s="11"/>
     </row>
     <row r="13" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B13" s="15" t="s">
+      <c r="B13" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="C13" s="15"/>
-      <c r="D13" s="15"/>
-      <c r="E13" s="15"/>
-      <c r="F13" s="15"/>
-      <c r="G13" s="15"/>
-      <c r="H13" s="15"/>
-      <c r="I13" s="15"/>
+      <c r="C13" s="11"/>
+      <c r="D13" s="11"/>
+      <c r="E13" s="11"/>
+      <c r="F13" s="11"/>
+      <c r="G13" s="11"/>
+      <c r="H13" s="11"/>
+      <c r="I13" s="11"/>
     </row>
     <row r="14" spans="2:9" x14ac:dyDescent="0.25">
       <c r="C14" s="4"/>
       <c r="D14" s="4"/>
     </row>
     <row r="15" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="C15" s="24"/>
-      <c r="D15" s="24"/>
-      <c r="G15" s="24"/>
-      <c r="H15" s="24"/>
+      <c r="C15" s="14"/>
+      <c r="D15" s="14"/>
+      <c r="G15" s="14"/>
+      <c r="H15" s="14"/>
     </row>
     <row r="16" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="C16" s="22" t="s">
+      <c r="C16" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="D16" s="22"/>
+      <c r="D16" s="12"/>
       <c r="E16" s="6"/>
       <c r="F16" s="6"/>
-      <c r="G16" s="22" t="s">
+      <c r="G16" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="H16" s="22"/>
+      <c r="H16" s="12"/>
     </row>
     <row r="17" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C17" s="23" t="s">
+      <c r="C17" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="D17" s="23"/>
-      <c r="G17" s="23" t="s">
+      <c r="D17" s="13"/>
+      <c r="G17" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="H17" s="23"/>
+      <c r="H17" s="13"/>
     </row>
   </sheetData>
   <mergeCells count="23">
+    <mergeCell ref="G8:I8"/>
+    <mergeCell ref="B8:F8"/>
+    <mergeCell ref="E9:I9"/>
+    <mergeCell ref="B9:D9"/>
+    <mergeCell ref="B10:D10"/>
+    <mergeCell ref="E10:I10"/>
+    <mergeCell ref="H2:H4"/>
+    <mergeCell ref="C2:C4"/>
+    <mergeCell ref="D2:F4"/>
+    <mergeCell ref="G2:G3"/>
+    <mergeCell ref="G6:H6"/>
+    <mergeCell ref="C6:F6"/>
     <mergeCell ref="B11:D11"/>
     <mergeCell ref="E11:I11"/>
     <mergeCell ref="C16:D16"/>
@@ -1291,18 +1327,6 @@
     <mergeCell ref="G15:H15"/>
     <mergeCell ref="G16:H16"/>
     <mergeCell ref="G17:H17"/>
-    <mergeCell ref="H2:H4"/>
-    <mergeCell ref="C2:C4"/>
-    <mergeCell ref="D2:F4"/>
-    <mergeCell ref="G2:G3"/>
-    <mergeCell ref="G6:H6"/>
-    <mergeCell ref="C6:F6"/>
-    <mergeCell ref="G8:I8"/>
-    <mergeCell ref="B8:F8"/>
-    <mergeCell ref="E9:I9"/>
-    <mergeCell ref="B9:D9"/>
-    <mergeCell ref="B10:D10"/>
-    <mergeCell ref="E10:I10"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -1312,67 +1336,67 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:T11"/>
+  <dimension ref="A2:S11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J2" sqref="J2:J4"/>
+    <sheetView tabSelected="1" topLeftCell="O1" workbookViewId="0">
+      <selection activeCell="U8" sqref="U8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="3" style="2" customWidth="1"/>
-    <col min="2" max="2" width="6" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.5703125" style="2" customWidth="1"/>
-    <col min="4" max="4" width="12" style="2" customWidth="1"/>
-    <col min="5" max="5" width="12.85546875" style="2" customWidth="1"/>
-    <col min="6" max="6" width="14.140625" style="2" customWidth="1"/>
-    <col min="7" max="7" width="12.140625" style="2" customWidth="1"/>
-    <col min="8" max="8" width="13.140625" style="2" customWidth="1"/>
-    <col min="9" max="9" width="12.7109375" style="2" customWidth="1"/>
-    <col min="10" max="10" width="11.42578125" style="2"/>
-    <col min="11" max="11" width="26.85546875" style="2" customWidth="1"/>
-    <col min="12" max="16" width="30.7109375" style="2" customWidth="1"/>
-    <col min="17" max="17" width="34.7109375" style="2" customWidth="1"/>
-    <col min="18" max="20" width="30.7109375" style="2" customWidth="1"/>
-    <col min="21" max="16384" width="11.42578125" style="2"/>
+    <col min="1" max="1" width="6" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.5703125" style="2" customWidth="1"/>
+    <col min="3" max="3" width="12" style="2" customWidth="1"/>
+    <col min="4" max="4" width="12.85546875" style="2" customWidth="1"/>
+    <col min="5" max="5" width="14.140625" style="2" customWidth="1"/>
+    <col min="6" max="6" width="12.140625" style="2" customWidth="1"/>
+    <col min="7" max="7" width="13.140625" style="2" customWidth="1"/>
+    <col min="8" max="8" width="12.7109375" style="2" customWidth="1"/>
+    <col min="9" max="9" width="11.42578125" style="2"/>
+    <col min="10" max="10" width="26.85546875" style="2" customWidth="1"/>
+    <col min="11" max="15" width="30.7109375" style="2" customWidth="1"/>
+    <col min="16" max="16" width="34.7109375" style="2" customWidth="1"/>
+    <col min="17" max="19" width="30.7109375" style="2" customWidth="1"/>
+    <col min="20" max="16384" width="11.42578125" style="2"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="D2" s="17"/>
-      <c r="E2" s="20" t="s">
+    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="C2" s="16"/>
+      <c r="D2" s="19" t="s">
         <v>2</v>
       </c>
-      <c r="F2" s="20"/>
-      <c r="G2" s="20"/>
-      <c r="H2" s="32" t="s">
+      <c r="E2" s="19"/>
+      <c r="F2" s="19"/>
+      <c r="G2" s="22" t="s">
         <v>42</v>
       </c>
-      <c r="I2" s="33"/>
-      <c r="J2" s="16"/>
-    </row>
-    <row r="3" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="D3" s="18"/>
-      <c r="E3" s="20"/>
-      <c r="F3" s="20"/>
-      <c r="G3" s="20"/>
-      <c r="H3" s="32" t="s">
+      <c r="H2" s="23"/>
+      <c r="I2" s="15"/>
+    </row>
+    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="C3" s="17"/>
+      <c r="D3" s="19"/>
+      <c r="E3" s="19"/>
+      <c r="F3" s="19"/>
+      <c r="G3" s="22" t="s">
         <v>40</v>
       </c>
-      <c r="I3" s="33"/>
-      <c r="J3" s="16"/>
-    </row>
-    <row r="4" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="H3" s="23"/>
+      <c r="I3" s="15"/>
+    </row>
+    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="C4" s="18"/>
       <c r="D4" s="19"/>
-      <c r="E4" s="20"/>
-      <c r="F4" s="20"/>
-      <c r="G4" s="20"/>
-      <c r="H4" s="32" t="s">
+      <c r="E4" s="19"/>
+      <c r="F4" s="19"/>
+      <c r="G4" s="22" t="s">
         <v>1</v>
       </c>
-      <c r="I4" s="33"/>
-      <c r="J4" s="16"/>
-    </row>
-    <row r="5" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="H4" s="23"/>
+      <c r="I4" s="15"/>
+    </row>
+    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="B5" s="8"/>
       <c r="C5" s="8"/>
       <c r="D5" s="8"/>
       <c r="E5" s="8"/>
@@ -1380,24 +1404,24 @@
       <c r="G5" s="8"/>
       <c r="H5" s="8"/>
       <c r="I5" s="8"/>
-      <c r="J5" s="8"/>
-    </row>
-    <row r="6" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="C6" s="15" t="s">
+    </row>
+    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="B6" s="11" t="s">
         <v>41</v>
       </c>
-      <c r="D6" s="15"/>
-      <c r="E6" s="15"/>
-      <c r="F6" s="15"/>
-      <c r="G6" s="15"/>
-      <c r="H6" s="15" t="s">
+      <c r="C6" s="11"/>
+      <c r="D6" s="11"/>
+      <c r="E6" s="11"/>
+      <c r="F6" s="11"/>
+      <c r="G6" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="I6" s="15"/>
-      <c r="J6" s="15"/>
-    </row>
-    <row r="7" spans="2:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="9"/>
+      <c r="H6" s="11"/>
+      <c r="I6" s="11"/>
+    </row>
+    <row r="7" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="9"/>
+      <c r="B7" s="7"/>
       <c r="C7" s="7"/>
       <c r="D7" s="7"/>
       <c r="E7" s="7"/>
@@ -1405,185 +1429,184 @@
       <c r="G7" s="7"/>
       <c r="H7" s="7"/>
       <c r="I7" s="7"/>
-      <c r="J7" s="7"/>
-      <c r="K7" s="9"/>
-      <c r="Q7" s="13" t="s">
+      <c r="J7" s="9"/>
+      <c r="P7" s="10" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="8" spans="2:20" s="10" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="B8" s="11" t="s">
+    <row r="8" spans="1:19" s="64" customFormat="1" ht="24" x14ac:dyDescent="0.25">
+      <c r="A8" s="61" t="s">
         <v>15</v>
       </c>
-      <c r="C8" s="25" t="s">
+      <c r="B8" s="62" t="s">
         <v>16</v>
       </c>
-      <c r="D8" s="25"/>
-      <c r="E8" s="25" t="s">
+      <c r="C8" s="62"/>
+      <c r="D8" s="62" t="s">
         <v>17</v>
       </c>
-      <c r="F8" s="25"/>
-      <c r="G8" s="11" t="s">
+      <c r="E8" s="62"/>
+      <c r="F8" s="61" t="s">
         <v>18</v>
       </c>
-      <c r="H8" s="25" t="s">
+      <c r="G8" s="62" t="s">
         <v>19</v>
       </c>
-      <c r="I8" s="25"/>
-      <c r="J8" s="25" t="s">
+      <c r="H8" s="62"/>
+      <c r="I8" s="62" t="s">
         <v>30</v>
       </c>
-      <c r="K8" s="25"/>
-      <c r="L8" s="12" t="s">
+      <c r="J8" s="62"/>
+      <c r="K8" s="63" t="s">
         <v>20</v>
       </c>
-      <c r="M8" s="12" t="s">
+      <c r="L8" s="63" t="s">
         <v>21</v>
       </c>
-      <c r="N8" s="12" t="s">
+      <c r="M8" s="63" t="s">
         <v>22</v>
       </c>
-      <c r="O8" s="12" t="s">
+      <c r="N8" s="63" t="s">
         <v>23</v>
       </c>
-      <c r="P8" s="12" t="s">
+      <c r="O8" s="63" t="s">
         <v>24</v>
       </c>
-      <c r="Q8" s="12" t="s">
+      <c r="P8" s="63" t="s">
         <v>25</v>
       </c>
-      <c r="R8" s="12" t="s">
+      <c r="Q8" s="63" t="s">
         <v>27</v>
       </c>
-      <c r="S8" s="12" t="s">
+      <c r="R8" s="63" t="s">
         <v>28</v>
       </c>
-      <c r="T8" s="12" t="s">
+      <c r="S8" s="63" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="9" spans="2:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="34">
+    <row r="9" spans="1:19" s="36" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="24">
         <v>1</v>
       </c>
-      <c r="C9" s="37" t="s">
+      <c r="B9" s="25" t="s">
         <v>34</v>
       </c>
-      <c r="D9" s="38"/>
-      <c r="E9" s="43" t="s">
+      <c r="C9" s="26"/>
+      <c r="D9" s="27" t="s">
         <v>35</v>
       </c>
-      <c r="F9" s="44"/>
-      <c r="G9" s="49">
+      <c r="E9" s="28"/>
+      <c r="F9" s="29">
         <v>42703</v>
       </c>
-      <c r="H9" s="52" t="s">
+      <c r="G9" s="30" t="s">
         <v>36</v>
       </c>
-      <c r="I9" s="53"/>
-      <c r="J9" s="26" t="s">
+      <c r="H9" s="31"/>
+      <c r="I9" s="32" t="s">
         <v>39</v>
       </c>
-      <c r="K9" s="27"/>
-      <c r="L9" s="61" t="s">
+      <c r="J9" s="33"/>
+      <c r="K9" s="34" t="s">
         <v>37</v>
       </c>
-      <c r="M9" s="61" t="s">
+      <c r="L9" s="34" t="s">
         <v>38</v>
       </c>
-      <c r="N9" s="58" t="s">
+      <c r="M9" s="35" t="s">
         <v>31</v>
       </c>
-      <c r="O9" s="58" t="s">
+      <c r="N9" s="35" t="s">
         <v>31</v>
       </c>
-      <c r="P9" s="58" t="s">
+      <c r="O9" s="35" t="s">
         <v>31</v>
       </c>
-      <c r="Q9" s="58" t="s">
+      <c r="P9" s="35" t="s">
         <v>32</v>
       </c>
-      <c r="R9" s="58" t="s">
+      <c r="Q9" s="35" t="s">
         <v>33</v>
       </c>
-      <c r="S9" s="49">
+      <c r="R9" s="29">
         <v>42704</v>
       </c>
-      <c r="T9" s="58" t="s">
+      <c r="S9" s="35" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="10" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B10" s="35"/>
+    <row r="10" spans="1:19" s="36" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
+      <c r="A10" s="37"/>
+      <c r="B10" s="38"/>
       <c r="C10" s="39"/>
       <c r="D10" s="40"/>
-      <c r="E10" s="45"/>
-      <c r="F10" s="46"/>
-      <c r="G10" s="50"/>
-      <c r="H10" s="54"/>
-      <c r="I10" s="55"/>
-      <c r="J10" s="28"/>
-      <c r="K10" s="29"/>
-      <c r="L10" s="62"/>
-      <c r="M10" s="62"/>
-      <c r="N10" s="59"/>
-      <c r="O10" s="59"/>
-      <c r="P10" s="59"/>
-      <c r="Q10" s="59"/>
-      <c r="R10" s="59"/>
-      <c r="S10" s="50"/>
-      <c r="T10" s="59"/>
-    </row>
-    <row r="11" spans="2:20" ht="57.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B11" s="36"/>
-      <c r="C11" s="41"/>
-      <c r="D11" s="42"/>
-      <c r="E11" s="47"/>
-      <c r="F11" s="48"/>
-      <c r="G11" s="51"/>
+      <c r="E10" s="41"/>
+      <c r="F10" s="42"/>
+      <c r="G10" s="43"/>
+      <c r="H10" s="44"/>
+      <c r="I10" s="45"/>
+      <c r="J10" s="46"/>
+      <c r="K10" s="47"/>
+      <c r="L10" s="47"/>
+      <c r="M10" s="48"/>
+      <c r="N10" s="48"/>
+      <c r="O10" s="48"/>
+      <c r="P10" s="48"/>
+      <c r="Q10" s="48"/>
+      <c r="R10" s="42"/>
+      <c r="S10" s="48"/>
+    </row>
+    <row r="11" spans="1:19" s="36" customFormat="1" ht="57.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A11" s="49"/>
+      <c r="B11" s="50"/>
+      <c r="C11" s="51"/>
+      <c r="D11" s="52"/>
+      <c r="E11" s="53"/>
+      <c r="F11" s="54"/>
+      <c r="G11" s="55"/>
       <c r="H11" s="56"/>
       <c r="I11" s="57"/>
-      <c r="J11" s="30"/>
-      <c r="K11" s="31"/>
-      <c r="L11" s="63"/>
-      <c r="M11" s="63"/>
+      <c r="J11" s="58"/>
+      <c r="K11" s="59"/>
+      <c r="L11" s="59"/>
+      <c r="M11" s="60"/>
       <c r="N11" s="60"/>
       <c r="O11" s="60"/>
       <c r="P11" s="60"/>
       <c r="Q11" s="60"/>
-      <c r="R11" s="60"/>
-      <c r="S11" s="51"/>
-      <c r="T11" s="60"/>
+      <c r="R11" s="54"/>
+      <c r="S11" s="60"/>
     </row>
   </sheetData>
   <mergeCells count="27">
+    <mergeCell ref="I8:J8"/>
+    <mergeCell ref="B8:C8"/>
+    <mergeCell ref="D8:E8"/>
+    <mergeCell ref="G8:H8"/>
+    <mergeCell ref="I9:J11"/>
+    <mergeCell ref="B6:F6"/>
+    <mergeCell ref="G6:I6"/>
+    <mergeCell ref="C2:C4"/>
+    <mergeCell ref="D2:F4"/>
+    <mergeCell ref="I2:I4"/>
+    <mergeCell ref="G2:H2"/>
+    <mergeCell ref="G3:H3"/>
+    <mergeCell ref="G4:H4"/>
+    <mergeCell ref="A9:A11"/>
+    <mergeCell ref="B9:C11"/>
+    <mergeCell ref="D9:E11"/>
+    <mergeCell ref="F9:F11"/>
+    <mergeCell ref="G9:H11"/>
+    <mergeCell ref="R9:R11"/>
     <mergeCell ref="S9:S11"/>
-    <mergeCell ref="T9:T11"/>
+    <mergeCell ref="K9:K11"/>
     <mergeCell ref="L9:L11"/>
+    <mergeCell ref="P9:P11"/>
+    <mergeCell ref="Q9:Q11"/>
     <mergeCell ref="M9:M11"/>
-    <mergeCell ref="Q9:Q11"/>
-    <mergeCell ref="R9:R11"/>
     <mergeCell ref="N9:N11"/>
     <mergeCell ref="O9:O11"/>
-    <mergeCell ref="P9:P11"/>
-    <mergeCell ref="B9:B11"/>
-    <mergeCell ref="C9:D11"/>
-    <mergeCell ref="E9:F11"/>
-    <mergeCell ref="G9:G11"/>
-    <mergeCell ref="H9:I11"/>
-    <mergeCell ref="C6:G6"/>
-    <mergeCell ref="H6:J6"/>
-    <mergeCell ref="D2:D4"/>
-    <mergeCell ref="E2:G4"/>
-    <mergeCell ref="J2:J4"/>
-    <mergeCell ref="H2:I2"/>
-    <mergeCell ref="H3:I3"/>
-    <mergeCell ref="H4:I4"/>
-    <mergeCell ref="J8:K8"/>
-    <mergeCell ref="C8:D8"/>
-    <mergeCell ref="E8:F8"/>
-    <mergeCell ref="H8:I8"/>
-    <mergeCell ref="J9:K11"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>